<commit_message>
Add aansluiting and bugfix dubbel results in table
</commit_message>
<xml_diff>
--- a/metadata/levels.xlsx
+++ b/metadata/levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahtanjung/Projects/ceda-fairnessawareness/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF10857-A09D-8E46-B370-C499D4B197E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F819B31-01F3-1345-A0AB-1397C82CC07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{CF7F6408-46E3-A244-99FB-EB7CAF439EE0}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
   <si>
     <t>MBO</t>
   </si>
@@ -140,6 +140,45 @@
   </si>
   <si>
     <t>aansluiting</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>studenten die direct na hun vooropleiding instromen</t>
+  </si>
+  <si>
+    <t>Tussenjaar</t>
+  </si>
+  <si>
+    <t>studenten met een of meer tussenjaren</t>
+  </si>
+  <si>
+    <t>Switch intern</t>
+  </si>
+  <si>
+    <t>interne switchers</t>
+  </si>
+  <si>
+    <t>Switch extern</t>
+  </si>
+  <si>
+    <t>externe switchers</t>
+  </si>
+  <si>
+    <t>2e Studie</t>
+  </si>
+  <si>
+    <t>studenten die twee of meer studies volgen</t>
+  </si>
+  <si>
+    <t>Na CD</t>
+  </si>
+  <si>
+    <t>studenten met een overige aansluiting</t>
+  </si>
+  <si>
+    <t>studenten met een onbekende aansluiting</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C288B8-7759-C849-A4AC-FBFBA106FE29}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1270,6 +1309,185 @@
       <c r="A12" t="s">
         <v>39</v>
       </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>